<commit_message>
Complete tools - TOT
</commit_message>
<xml_diff>
--- a/Kingdom/KingdomSimulator.xlsx
+++ b/Kingdom/KingdomSimulator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/Kingdom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838879FF-FE2A-694C-AC7B-7222BD3D65E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65969DF-CA38-7D48-A20D-3324FF496E44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{7FFFBABC-6793-4F48-8984-0BF1F567D385}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{7FFFBABC-6793-4F48-8984-0BF1F567D385}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="110">
   <si>
     <t>BAT3</t>
   </si>
@@ -338,6 +338,33 @@
   <si>
     <t>每第一次升段之后赠送盾*1</t>
   </si>
+  <si>
+    <t>目前只配纯活跃向的任务</t>
+  </si>
+  <si>
+    <t>活跃条件-数据</t>
+  </si>
+  <si>
+    <t>输了不扣</t>
+  </si>
+  <si>
+    <t>任务3 「buff」</t>
+  </si>
+  <si>
+    <t>任务2 「双倍卡 or 盾 」</t>
+  </si>
+  <si>
+    <t>小活</t>
+  </si>
+  <si>
+    <t>中活</t>
+  </si>
+  <si>
+    <t>高活</t>
+  </si>
+  <si>
+    <t>任务1[ 奖励]</t>
+  </si>
 </sst>
 </file>
 
@@ -374,7 +401,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,6 +417,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -421,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -430,11 +469,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1008FC5-4C04-EE4B-A35B-C84E380B5767}">
   <dimension ref="A1:BC1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -761,40 +803,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55">
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="8"/>
-      <c r="AN1" s="8"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="8"/>
-      <c r="AQ1" s="8"/>
-      <c r="AR1" s="8"/>
-      <c r="AS1" s="8"/>
-      <c r="AT1" s="8"/>
-      <c r="AU1" s="8"/>
-      <c r="AV1" s="8"/>
-      <c r="AW1" s="8"/>
-      <c r="AX1" s="8"/>
-      <c r="AY1" s="8"/>
-      <c r="AZ1" s="8"/>
-      <c r="BA1" s="8"/>
-      <c r="BB1" s="8"/>
-      <c r="BC1" s="8"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AD1" s="10"/>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="10"/>
+      <c r="AI1" s="10"/>
+      <c r="AJ1" s="10"/>
+      <c r="AK1" s="10"/>
+      <c r="AL1" s="10"/>
+      <c r="AM1" s="10"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
+      <c r="AP1" s="10"/>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="10"/>
     </row>
     <row r="2" spans="1:55">
       <c r="A2" s="1"/>
@@ -946,25 +988,25 @@
       <c r="D5" s="6">
         <v>0.5</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>0.38938842346886499</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>0.23240303306998999</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0.121077935222672</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="8">
         <v>5.4166666666666599E-2</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="9">
         <v>1.694915E-2</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>0</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <v>0</v>
       </c>
       <c r="L5" s="1"/>
@@ -987,8 +1029,10 @@
         <v>8</v>
       </c>
       <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="1"/>
+      <c r="V5" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="W5" s="12"/>
       <c r="X5" t="s">
         <v>72</v>
       </c>
@@ -1091,28 +1135,28 @@
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>0.61061157653113396</v>
       </c>
       <c r="E6" s="6">
         <v>0.5</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <v>0.31754829433454601</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>0.19900250614128601</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="8">
         <v>0.110471929263875</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <v>6.6095471236230094E-2</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>0</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="8">
         <v>0</v>
       </c>
       <c r="L6" s="1"/>
@@ -1135,10 +1179,14 @@
         <v>10</v>
       </c>
       <c r="U6" s="2"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
+      <c r="V6" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="W6" t="s">
+        <v>106</v>
+      </c>
       <c r="X6" s="1" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="Y6" s="2">
         <v>3</v>
@@ -1239,25 +1287,25 @@
       <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>0.76759696693000901</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>0.68246330094385499</v>
       </c>
       <c r="F7" s="6">
         <v>0.5</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>0.34141425942693499</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="8">
         <v>0.208795117211068</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>0.13136309825807499</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>0.110878661087866</v>
       </c>
       <c r="K7" s="4">
@@ -1284,9 +1332,11 @@
       </c>
       <c r="U7" s="2"/>
       <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
+      <c r="W7" s="1" t="s">
+        <v>107</v>
+      </c>
       <c r="X7" s="1" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="Y7" s="2">
         <v>3</v>
@@ -1428,9 +1478,11 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
+      <c r="W8" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="X8" s="1" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="Y8" s="2">
         <v>5</v>
@@ -1820,22 +1872,99 @@
       <c r="X12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Y12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AC12" s="2"/>
-      <c r="AE12" s="2"/>
-      <c r="AG12" s="2"/>
-      <c r="AI12" s="2"/>
-      <c r="AK12" s="2"/>
-      <c r="AM12" s="2"/>
-      <c r="AO12" s="2"/>
-      <c r="AQ12" s="2"/>
-      <c r="AS12" s="2"/>
-      <c r="AU12" s="2"/>
-      <c r="AW12" s="2"/>
-      <c r="AY12" s="2"/>
-      <c r="BA12" s="2"/>
-      <c r="BC12" s="2"/>
+      <c r="Y12" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z12">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB12">
+        <v>3</v>
+      </c>
+      <c r="AC12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+      <c r="AE12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF12">
+        <v>3</v>
+      </c>
+      <c r="AG12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH12">
+        <v>3</v>
+      </c>
+      <c r="AI12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ12">
+        <v>3</v>
+      </c>
+      <c r="AK12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL12">
+        <v>3</v>
+      </c>
+      <c r="AM12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN12">
+        <v>3</v>
+      </c>
+      <c r="AO12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AP12">
+        <v>3</v>
+      </c>
+      <c r="AQ12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AR12">
+        <v>3</v>
+      </c>
+      <c r="AS12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AT12">
+        <v>3</v>
+      </c>
+      <c r="AU12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AV12">
+        <v>3</v>
+      </c>
+      <c r="AW12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AX12">
+        <v>3</v>
+      </c>
+      <c r="AY12" s="2">
+        <v>3</v>
+      </c>
+      <c r="AZ12">
+        <v>3</v>
+      </c>
+      <c r="BA12" s="2">
+        <v>3</v>
+      </c>
+      <c r="BB12">
+        <v>3</v>
+      </c>
+      <c r="BC12" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:55">
       <c r="A13" s="1"/>
@@ -1870,22 +1999,99 @@
       <c r="X13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Y13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AE13" s="2"/>
-      <c r="AG13" s="2"/>
-      <c r="AI13" s="2"/>
-      <c r="AK13" s="2"/>
-      <c r="AM13" s="2"/>
-      <c r="AO13" s="2"/>
-      <c r="AQ13" s="2"/>
-      <c r="AS13" s="2"/>
-      <c r="AU13" s="2"/>
-      <c r="AW13" s="2"/>
-      <c r="AY13" s="2"/>
-      <c r="BA13" s="2"/>
-      <c r="BC13" s="2"/>
+      <c r="Y13" s="2">
+        <v>3</v>
+      </c>
+      <c r="Z13">
+        <v>3</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB13">
+        <v>3</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AD13">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AF13">
+        <v>3</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH13">
+        <v>3</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AJ13">
+        <v>3</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AL13">
+        <v>3</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN13">
+        <v>3</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AP13">
+        <v>3</v>
+      </c>
+      <c r="AQ13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AR13">
+        <v>3</v>
+      </c>
+      <c r="AS13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AT13">
+        <v>3</v>
+      </c>
+      <c r="AU13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AV13">
+        <v>3</v>
+      </c>
+      <c r="AW13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AX13">
+        <v>3</v>
+      </c>
+      <c r="AY13" s="2">
+        <v>3</v>
+      </c>
+      <c r="AZ13">
+        <v>3</v>
+      </c>
+      <c r="BA13" s="2">
+        <v>3</v>
+      </c>
+      <c r="BB13">
+        <v>3</v>
+      </c>
+      <c r="BC13" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:55">
       <c r="A14" s="1"/>
@@ -1924,22 +2130,99 @@
       <c r="X14" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Y14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AG14" s="2"/>
-      <c r="AI14" s="2"/>
-      <c r="AK14" s="2"/>
-      <c r="AM14" s="2"/>
-      <c r="AO14" s="2"/>
-      <c r="AQ14" s="2"/>
-      <c r="AS14" s="2"/>
-      <c r="AU14" s="2"/>
-      <c r="AW14" s="2"/>
-      <c r="AY14" s="2"/>
-      <c r="BA14" s="2"/>
-      <c r="BC14" s="2"/>
+      <c r="Y14" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z14">
+        <v>5</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AB14">
+        <v>5</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AD14">
+        <v>5</v>
+      </c>
+      <c r="AE14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AF14">
+        <v>5</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AH14">
+        <v>5</v>
+      </c>
+      <c r="AI14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AJ14">
+        <v>5</v>
+      </c>
+      <c r="AK14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AL14">
+        <v>5</v>
+      </c>
+      <c r="AM14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AN14">
+        <v>5</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AP14">
+        <v>5</v>
+      </c>
+      <c r="AQ14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AR14">
+        <v>5</v>
+      </c>
+      <c r="AS14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AT14">
+        <v>5</v>
+      </c>
+      <c r="AU14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AV14">
+        <v>5</v>
+      </c>
+      <c r="AW14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AX14">
+        <v>5</v>
+      </c>
+      <c r="AY14" s="2">
+        <v>5</v>
+      </c>
+      <c r="AZ14">
+        <v>5</v>
+      </c>
+      <c r="BA14" s="2">
+        <v>5</v>
+      </c>
+      <c r="BB14">
+        <v>5</v>
+      </c>
+      <c r="BC14" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:55">
       <c r="A15" s="1"/>
@@ -2058,7 +2341,9 @@
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
+      <c r="W17" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="X17" t="s">
         <v>82</v>
       </c>
@@ -2164,14 +2449,30 @@
       <c r="C18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
+      <c r="D18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K18" s="1">
+        <v>1000</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="2" t="s">
@@ -2193,23 +2494,98 @@
         <v>67</v>
       </c>
       <c r="Y18" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="AA18" s="2"/>
-      <c r="AC18" s="2"/>
-      <c r="AE18" s="2"/>
-      <c r="AG18" s="2"/>
-      <c r="AI18" s="2"/>
-      <c r="AK18" s="2"/>
-      <c r="AM18" s="2"/>
-      <c r="AO18" s="2"/>
-      <c r="AQ18" s="2"/>
-      <c r="AS18" s="2"/>
-      <c r="AU18" s="2"/>
-      <c r="AW18" s="2"/>
-      <c r="AY18" s="2"/>
-      <c r="BA18" s="2"/>
-      <c r="BC18" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AA18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AB18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AC18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AD18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AE18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AF18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AG18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AH18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AI18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AJ18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AL18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AM18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AN18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AO18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AP18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AQ18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AR18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AS18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AT18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AU18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AV18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AW18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AX18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AY18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AZ18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BA18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BB18" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BC18" s="2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="19" spans="1:55">
       <c r="A19" s="1"/>
@@ -2219,14 +2595,30 @@
       <c r="C19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+      <c r="D19" s="1">
+        <v>900</v>
+      </c>
+      <c r="E19" s="1">
+        <v>900</v>
+      </c>
+      <c r="F19" s="1">
+        <v>900</v>
+      </c>
+      <c r="G19" s="1">
+        <v>900</v>
+      </c>
+      <c r="H19" s="1">
+        <v>900</v>
+      </c>
+      <c r="I19" s="1">
+        <v>900</v>
+      </c>
+      <c r="J19" s="1">
+        <v>900</v>
+      </c>
+      <c r="K19" s="1">
+        <v>900</v>
+      </c>
       <c r="L19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="2" t="s">
@@ -2248,23 +2640,98 @@
         <v>68</v>
       </c>
       <c r="Y19" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="2"/>
-      <c r="AC19" s="2"/>
-      <c r="AE19" s="2"/>
-      <c r="AG19" s="2"/>
-      <c r="AI19" s="2"/>
-      <c r="AK19" s="2"/>
-      <c r="AM19" s="2"/>
-      <c r="AO19" s="2"/>
-      <c r="AQ19" s="2"/>
-      <c r="AS19" s="2"/>
-      <c r="AU19" s="2"/>
-      <c r="AW19" s="2"/>
-      <c r="AY19" s="2"/>
-      <c r="BA19" s="2"/>
-      <c r="BC19" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AA19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AB19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AC19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AD19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AE19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AF19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AG19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AH19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AI19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AJ19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AK19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AL19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AM19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AN19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AO19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AP19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AQ19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AR19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AS19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AT19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AU19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AV19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AW19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AX19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AY19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AZ19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BA19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BB19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BC19" s="2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="20" spans="1:55">
       <c r="A20" s="1"/>
@@ -2274,14 +2741,30 @@
       <c r="C20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="D20" s="1">
+        <v>800</v>
+      </c>
+      <c r="E20" s="1">
+        <v>800</v>
+      </c>
+      <c r="F20" s="1">
+        <v>800</v>
+      </c>
+      <c r="G20" s="1">
+        <v>800</v>
+      </c>
+      <c r="H20" s="1">
+        <v>800</v>
+      </c>
+      <c r="I20" s="1">
+        <v>800</v>
+      </c>
+      <c r="J20" s="1">
+        <v>800</v>
+      </c>
+      <c r="K20" s="1">
+        <v>800</v>
+      </c>
       <c r="L20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="2" t="s">
@@ -2305,21 +2788,96 @@
       <c r="Y20" s="2">
         <v>0.2</v>
       </c>
-      <c r="AA20" s="2"/>
-      <c r="AC20" s="2"/>
-      <c r="AE20" s="2"/>
-      <c r="AG20" s="2"/>
-      <c r="AI20" s="2"/>
-      <c r="AK20" s="2"/>
-      <c r="AM20" s="2"/>
-      <c r="AO20" s="2"/>
-      <c r="AQ20" s="2"/>
-      <c r="AS20" s="2"/>
-      <c r="AU20" s="2"/>
-      <c r="AW20" s="2"/>
-      <c r="AY20" s="2"/>
-      <c r="BA20" s="2"/>
-      <c r="BC20" s="2"/>
+      <c r="Z20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AA20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AB20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AC20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AD20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AE20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AF20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AG20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AH20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AI20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AJ20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AK20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AL20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AM20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AN20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AO20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AP20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AQ20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AR20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AS20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AT20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AU20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AV20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AW20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AX20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AY20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AZ20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BA20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BB20" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BC20" s="2">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="21" spans="1:55">
       <c r="A21" s="1"/>
@@ -2329,14 +2887,30 @@
       <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
+      <c r="D21" s="1">
+        <v>700</v>
+      </c>
+      <c r="E21" s="1">
+        <v>700</v>
+      </c>
+      <c r="F21" s="1">
+        <v>700</v>
+      </c>
+      <c r="G21" s="1">
+        <v>700</v>
+      </c>
+      <c r="H21" s="1">
+        <v>700</v>
+      </c>
+      <c r="I21" s="1">
+        <v>700</v>
+      </c>
+      <c r="J21" s="1">
+        <v>700</v>
+      </c>
+      <c r="K21" s="1">
+        <v>700</v>
+      </c>
       <c r="L21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="2" t="s">
@@ -2366,14 +2940,30 @@
       <c r="C22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
+      <c r="D22" s="1">
+        <v>600</v>
+      </c>
+      <c r="E22" s="1">
+        <v>600</v>
+      </c>
+      <c r="F22" s="1">
+        <v>600</v>
+      </c>
+      <c r="G22" s="1">
+        <v>600</v>
+      </c>
+      <c r="H22" s="1">
+        <v>600</v>
+      </c>
+      <c r="I22" s="1">
+        <v>600</v>
+      </c>
+      <c r="J22" s="1">
+        <v>600</v>
+      </c>
+      <c r="K22" s="1">
+        <v>600</v>
+      </c>
       <c r="L22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="2" t="s">
@@ -2407,14 +2997,30 @@
       <c r="C23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
+      <c r="D23" s="1">
+        <v>500</v>
+      </c>
+      <c r="E23" s="1">
+        <v>500</v>
+      </c>
+      <c r="F23" s="1">
+        <v>500</v>
+      </c>
+      <c r="G23" s="1">
+        <v>500</v>
+      </c>
+      <c r="H23" s="1">
+        <v>500</v>
+      </c>
+      <c r="I23" s="1">
+        <v>500</v>
+      </c>
+      <c r="J23" s="1">
+        <v>500</v>
+      </c>
+      <c r="K23" s="1">
+        <v>500</v>
+      </c>
       <c r="L23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="2" t="s">
@@ -2539,14 +3145,30 @@
       <c r="C24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
+      <c r="D24" s="1">
+        <v>400</v>
+      </c>
+      <c r="E24" s="1">
+        <v>400</v>
+      </c>
+      <c r="F24" s="1">
+        <v>400</v>
+      </c>
+      <c r="G24" s="1">
+        <v>400</v>
+      </c>
+      <c r="H24" s="1">
+        <v>400</v>
+      </c>
+      <c r="I24" s="1">
+        <v>400</v>
+      </c>
+      <c r="J24" s="1">
+        <v>400</v>
+      </c>
+      <c r="K24" s="1">
+        <v>400</v>
+      </c>
       <c r="L24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="2" t="s">
@@ -2592,14 +3214,30 @@
       <c r="C25" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
+      <c r="D25" s="1">
+        <v>300</v>
+      </c>
+      <c r="E25" s="1">
+        <v>300</v>
+      </c>
+      <c r="F25" s="1">
+        <v>300</v>
+      </c>
+      <c r="G25" s="1">
+        <v>300</v>
+      </c>
+      <c r="H25" s="1">
+        <v>300</v>
+      </c>
+      <c r="I25" s="1">
+        <v>300</v>
+      </c>
+      <c r="J25" s="1">
+        <v>300</v>
+      </c>
+      <c r="K25" s="1">
+        <v>300</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="2" t="s">
@@ -2645,14 +3283,30 @@
       <c r="C26" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
+      <c r="D26" s="1">
+        <v>200</v>
+      </c>
+      <c r="E26" s="1">
+        <v>200</v>
+      </c>
+      <c r="F26" s="1">
+        <v>200</v>
+      </c>
+      <c r="G26" s="1">
+        <v>200</v>
+      </c>
+      <c r="H26" s="1">
+        <v>200</v>
+      </c>
+      <c r="I26" s="1">
+        <v>200</v>
+      </c>
+      <c r="J26" s="1">
+        <v>200</v>
+      </c>
+      <c r="K26" s="1">
+        <v>200</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="2" t="s">
@@ -2775,14 +3429,30 @@
       <c r="C27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
+      <c r="D27" s="1">
+        <v>100</v>
+      </c>
+      <c r="E27" s="1">
+        <v>100</v>
+      </c>
+      <c r="F27" s="1">
+        <v>100</v>
+      </c>
+      <c r="G27" s="1">
+        <v>100</v>
+      </c>
+      <c r="H27" s="1">
+        <v>100</v>
+      </c>
+      <c r="I27" s="1">
+        <v>100</v>
+      </c>
+      <c r="J27" s="1">
+        <v>100</v>
+      </c>
+      <c r="K27" s="1">
+        <v>100</v>
+      </c>
       <c r="L27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="2" t="s">
@@ -2810,14 +3480,30 @@
       <c r="C28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
+      <c r="D28" s="1">
+        <v>100</v>
+      </c>
+      <c r="E28" s="1">
+        <v>100</v>
+      </c>
+      <c r="F28" s="1">
+        <v>100</v>
+      </c>
+      <c r="G28" s="1">
+        <v>100</v>
+      </c>
+      <c r="H28" s="1">
+        <v>100</v>
+      </c>
+      <c r="I28" s="1">
+        <v>100</v>
+      </c>
+      <c r="J28" s="1">
+        <v>100</v>
+      </c>
+      <c r="K28" s="1">
+        <v>100</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="2" t="s">
@@ -2846,14 +3532,30 @@
       <c r="C29" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
+      <c r="D29" s="1">
+        <v>100</v>
+      </c>
+      <c r="E29" s="1">
+        <v>100</v>
+      </c>
+      <c r="F29" s="1">
+        <v>100</v>
+      </c>
+      <c r="G29" s="1">
+        <v>100</v>
+      </c>
+      <c r="H29" s="1">
+        <v>100</v>
+      </c>
+      <c r="I29" s="1">
+        <v>100</v>
+      </c>
+      <c r="J29" s="1">
+        <v>100</v>
+      </c>
+      <c r="K29" s="1">
+        <v>100</v>
+      </c>
       <c r="L29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="2" t="s">
@@ -2888,14 +3590,30 @@
       <c r="C30" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
+      <c r="D30" s="1">
+        <v>100</v>
+      </c>
+      <c r="E30" s="1">
+        <v>100</v>
+      </c>
+      <c r="F30" s="1">
+        <v>100</v>
+      </c>
+      <c r="G30" s="1">
+        <v>100</v>
+      </c>
+      <c r="H30" s="1">
+        <v>100</v>
+      </c>
+      <c r="I30" s="1">
+        <v>100</v>
+      </c>
+      <c r="J30" s="1">
+        <v>100</v>
+      </c>
+      <c r="K30" s="1">
+        <v>100</v>
+      </c>
       <c r="L30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="2" t="s">
@@ -3018,14 +3736,30 @@
       <c r="C31" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
+      <c r="D31" s="1">
+        <v>100</v>
+      </c>
+      <c r="E31" s="1">
+        <v>100</v>
+      </c>
+      <c r="F31" s="1">
+        <v>100</v>
+      </c>
+      <c r="G31" s="1">
+        <v>100</v>
+      </c>
+      <c r="H31" s="1">
+        <v>100</v>
+      </c>
+      <c r="I31" s="1">
+        <v>100</v>
+      </c>
+      <c r="J31" s="1">
+        <v>100</v>
+      </c>
+      <c r="K31" s="1">
+        <v>100</v>
+      </c>
       <c r="L31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="2" t="s">
@@ -3047,23 +3781,98 @@
         <v>67</v>
       </c>
       <c r="Y31" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="AA31" s="2"/>
-      <c r="AC31" s="2"/>
-      <c r="AE31" s="2"/>
-      <c r="AG31" s="2"/>
-      <c r="AI31" s="2"/>
-      <c r="AK31" s="2"/>
-      <c r="AM31" s="2"/>
-      <c r="AO31" s="2"/>
-      <c r="AQ31" s="2"/>
-      <c r="AS31" s="2"/>
-      <c r="AU31" s="2"/>
-      <c r="AW31" s="2"/>
-      <c r="AY31" s="2"/>
-      <c r="BA31" s="2"/>
-      <c r="BC31" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AA31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AB31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AC31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AD31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AE31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AF31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AG31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AH31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AI31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AJ31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AK31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AL31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AM31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AN31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AO31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AP31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AQ31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AR31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AS31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AT31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AU31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AV31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AW31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AX31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AY31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="AZ31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BA31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BB31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="BC31" s="2">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="32" spans="1:55">
       <c r="A32" s="1"/>
@@ -3073,14 +3882,30 @@
       <c r="C32" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+      <c r="D32" s="1">
+        <v>100</v>
+      </c>
+      <c r="E32" s="1">
+        <v>100</v>
+      </c>
+      <c r="F32" s="1">
+        <v>100</v>
+      </c>
+      <c r="G32" s="1">
+        <v>100</v>
+      </c>
+      <c r="H32" s="1">
+        <v>100</v>
+      </c>
+      <c r="I32" s="1">
+        <v>100</v>
+      </c>
+      <c r="J32" s="1">
+        <v>100</v>
+      </c>
+      <c r="K32" s="1">
+        <v>100</v>
+      </c>
       <c r="L32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="2" t="s">
@@ -3102,23 +3927,98 @@
         <v>68</v>
       </c>
       <c r="Y32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA32" s="2"/>
-      <c r="AC32" s="2"/>
-      <c r="AE32" s="2"/>
-      <c r="AG32" s="2"/>
-      <c r="AI32" s="2"/>
-      <c r="AK32" s="2"/>
-      <c r="AM32" s="2"/>
-      <c r="AO32" s="2"/>
-      <c r="AQ32" s="2"/>
-      <c r="AS32" s="2"/>
-      <c r="AU32" s="2"/>
-      <c r="AW32" s="2"/>
-      <c r="AY32" s="2"/>
-      <c r="BA32" s="2"/>
-      <c r="BC32" s="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="Z32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AA32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AB32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AC32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AD32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AE32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AF32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AG32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AH32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AI32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AJ32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AK32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AL32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AM32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AN32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AO32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AP32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AQ32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AR32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AS32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AT32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AU32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AV32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AW32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AX32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AY32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AZ32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BA32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BB32" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BC32" s="2">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="33" spans="1:55">
       <c r="A33" s="1"/>
@@ -3128,14 +4028,30 @@
       <c r="C33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="D33" s="1">
+        <v>100</v>
+      </c>
+      <c r="E33" s="1">
+        <v>100</v>
+      </c>
+      <c r="F33" s="1">
+        <v>100</v>
+      </c>
+      <c r="G33" s="1">
+        <v>100</v>
+      </c>
+      <c r="H33" s="1">
+        <v>100</v>
+      </c>
+      <c r="I33" s="1">
+        <v>100</v>
+      </c>
+      <c r="J33" s="1">
+        <v>100</v>
+      </c>
+      <c r="K33" s="1">
+        <v>100</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -3153,21 +4069,96 @@
       <c r="Y33" s="2">
         <v>0.2</v>
       </c>
-      <c r="AA33" s="2"/>
-      <c r="AC33" s="2"/>
-      <c r="AE33" s="2"/>
-      <c r="AG33" s="2"/>
-      <c r="AI33" s="2"/>
-      <c r="AK33" s="2"/>
-      <c r="AM33" s="2"/>
-      <c r="AO33" s="2"/>
-      <c r="AQ33" s="2"/>
-      <c r="AS33" s="2"/>
-      <c r="AU33" s="2"/>
-      <c r="AW33" s="2"/>
-      <c r="AY33" s="2"/>
-      <c r="BA33" s="2"/>
-      <c r="BC33" s="2"/>
+      <c r="Z33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AA33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AB33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AC33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AD33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AE33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AF33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AG33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AH33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AI33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AJ33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AK33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AL33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AM33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AN33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AO33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AP33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AQ33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AR33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AS33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AT33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AU33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AV33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AW33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AX33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AY33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="AZ33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BA33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BB33" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="BC33" s="2">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="34" spans="1:55">
       <c r="A34" s="1"/>
@@ -3177,14 +4168,30 @@
       <c r="C34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
+      <c r="D34" s="1">
+        <v>100</v>
+      </c>
+      <c r="E34" s="1">
+        <v>100</v>
+      </c>
+      <c r="F34" s="1">
+        <v>100</v>
+      </c>
+      <c r="G34" s="1">
+        <v>100</v>
+      </c>
+      <c r="H34" s="1">
+        <v>100</v>
+      </c>
+      <c r="I34" s="1">
+        <v>100</v>
+      </c>
+      <c r="J34" s="1">
+        <v>100</v>
+      </c>
+      <c r="K34" s="1">
+        <v>100</v>
+      </c>
       <c r="L34" s="1"/>
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
@@ -3207,14 +4214,30 @@
       <c r="C35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
+      <c r="D35" s="1">
+        <v>100</v>
+      </c>
+      <c r="E35" s="1">
+        <v>100</v>
+      </c>
+      <c r="F35" s="1">
+        <v>100</v>
+      </c>
+      <c r="G35" s="1">
+        <v>100</v>
+      </c>
+      <c r="H35" s="1">
+        <v>100</v>
+      </c>
+      <c r="I35" s="1">
+        <v>100</v>
+      </c>
+      <c r="J35" s="1">
+        <v>100</v>
+      </c>
+      <c r="K35" s="1">
+        <v>100</v>
+      </c>
       <c r="L35" s="1"/>
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
@@ -3237,14 +4260,30 @@
       <c r="C36" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+      <c r="D36" s="1">
+        <v>100</v>
+      </c>
+      <c r="E36" s="1">
+        <v>100</v>
+      </c>
+      <c r="F36" s="1">
+        <v>100</v>
+      </c>
+      <c r="G36" s="1">
+        <v>100</v>
+      </c>
+      <c r="H36" s="1">
+        <v>100</v>
+      </c>
+      <c r="I36" s="1">
+        <v>100</v>
+      </c>
+      <c r="J36" s="1">
+        <v>100</v>
+      </c>
+      <c r="K36" s="1">
+        <v>100</v>
+      </c>
       <c r="L36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -3268,14 +4307,30 @@
       <c r="C37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
+      <c r="D37" s="1">
+        <v>100</v>
+      </c>
+      <c r="E37" s="1">
+        <v>100</v>
+      </c>
+      <c r="F37" s="1">
+        <v>100</v>
+      </c>
+      <c r="G37" s="1">
+        <v>100</v>
+      </c>
+      <c r="H37" s="1">
+        <v>100</v>
+      </c>
+      <c r="I37" s="1">
+        <v>100</v>
+      </c>
+      <c r="J37" s="1">
+        <v>100</v>
+      </c>
+      <c r="K37" s="1">
+        <v>100</v>
+      </c>
       <c r="L37" s="1"/>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
@@ -3299,14 +4354,30 @@
       <c r="C38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
+      <c r="D38" s="1">
+        <v>100</v>
+      </c>
+      <c r="E38" s="1">
+        <v>100</v>
+      </c>
+      <c r="F38" s="1">
+        <v>100</v>
+      </c>
+      <c r="G38" s="1">
+        <v>100</v>
+      </c>
+      <c r="H38" s="1">
+        <v>100</v>
+      </c>
+      <c r="I38" s="1">
+        <v>100</v>
+      </c>
+      <c r="J38" s="1">
+        <v>100</v>
+      </c>
+      <c r="K38" s="1">
+        <v>100</v>
+      </c>
       <c r="L38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -3330,14 +4401,30 @@
       <c r="C39" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
+      <c r="D39" s="1">
+        <v>100</v>
+      </c>
+      <c r="E39" s="1">
+        <v>100</v>
+      </c>
+      <c r="F39" s="1">
+        <v>100</v>
+      </c>
+      <c r="G39" s="1">
+        <v>100</v>
+      </c>
+      <c r="H39" s="1">
+        <v>100</v>
+      </c>
+      <c r="I39" s="1">
+        <v>100</v>
+      </c>
+      <c r="J39" s="1">
+        <v>100</v>
+      </c>
+      <c r="K39" s="1">
+        <v>100</v>
+      </c>
       <c r="L39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -3361,14 +4448,30 @@
       <c r="C40" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
+      <c r="D40" s="1">
+        <v>100</v>
+      </c>
+      <c r="E40" s="1">
+        <v>100</v>
+      </c>
+      <c r="F40" s="1">
+        <v>100</v>
+      </c>
+      <c r="G40" s="1">
+        <v>100</v>
+      </c>
+      <c r="H40" s="1">
+        <v>100</v>
+      </c>
+      <c r="I40" s="1">
+        <v>100</v>
+      </c>
+      <c r="J40" s="1">
+        <v>100</v>
+      </c>
+      <c r="K40" s="1">
+        <v>100</v>
+      </c>
       <c r="L40" s="1"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
@@ -3392,14 +4495,30 @@
       <c r="C41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
+      <c r="D41" s="1">
+        <v>100</v>
+      </c>
+      <c r="E41" s="1">
+        <v>100</v>
+      </c>
+      <c r="F41" s="1">
+        <v>100</v>
+      </c>
+      <c r="G41" s="1">
+        <v>100</v>
+      </c>
+      <c r="H41" s="1">
+        <v>100</v>
+      </c>
+      <c r="I41" s="1">
+        <v>100</v>
+      </c>
+      <c r="J41" s="1">
+        <v>100</v>
+      </c>
+      <c r="K41" s="1">
+        <v>100</v>
+      </c>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
@@ -3424,14 +4543,30 @@
       <c r="C42" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
+      <c r="D42" s="1">
+        <v>100</v>
+      </c>
+      <c r="E42" s="1">
+        <v>100</v>
+      </c>
+      <c r="F42" s="1">
+        <v>100</v>
+      </c>
+      <c r="G42" s="1">
+        <v>100</v>
+      </c>
+      <c r="H42" s="1">
+        <v>100</v>
+      </c>
+      <c r="I42" s="1">
+        <v>100</v>
+      </c>
+      <c r="J42" s="1">
+        <v>100</v>
+      </c>
+      <c r="K42" s="1">
+        <v>100</v>
+      </c>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -3456,14 +4591,30 @@
       <c r="C43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
+      <c r="D43" s="1">
+        <v>100</v>
+      </c>
+      <c r="E43" s="1">
+        <v>100</v>
+      </c>
+      <c r="F43" s="1">
+        <v>100</v>
+      </c>
+      <c r="G43" s="1">
+        <v>100</v>
+      </c>
+      <c r="H43" s="1">
+        <v>100</v>
+      </c>
+      <c r="I43" s="1">
+        <v>100</v>
+      </c>
+      <c r="J43" s="1">
+        <v>100</v>
+      </c>
+      <c r="K43" s="1">
+        <v>100</v>
+      </c>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -3488,14 +4639,30 @@
       <c r="C44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
+      <c r="D44" s="1">
+        <v>100</v>
+      </c>
+      <c r="E44" s="1">
+        <v>100</v>
+      </c>
+      <c r="F44" s="1">
+        <v>100</v>
+      </c>
+      <c r="G44" s="1">
+        <v>100</v>
+      </c>
+      <c r="H44" s="1">
+        <v>100</v>
+      </c>
+      <c r="I44" s="1">
+        <v>100</v>
+      </c>
+      <c r="J44" s="1">
+        <v>100</v>
+      </c>
+      <c r="K44" s="1">
+        <v>100</v>
+      </c>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
@@ -3520,14 +4687,30 @@
       <c r="C45" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
+      <c r="D45" s="1">
+        <v>100</v>
+      </c>
+      <c r="E45" s="1">
+        <v>100</v>
+      </c>
+      <c r="F45" s="1">
+        <v>100</v>
+      </c>
+      <c r="G45" s="1">
+        <v>100</v>
+      </c>
+      <c r="H45" s="1">
+        <v>100</v>
+      </c>
+      <c r="I45" s="1">
+        <v>100</v>
+      </c>
+      <c r="J45" s="1">
+        <v>100</v>
+      </c>
+      <c r="K45" s="1">
+        <v>100</v>
+      </c>
       <c r="L45" s="1"/>
       <c r="M45" s="2" t="s">
         <v>25</v>
@@ -3554,14 +4737,30 @@
       <c r="C46" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
+      <c r="D46" s="1">
+        <v>100</v>
+      </c>
+      <c r="E46" s="1">
+        <v>100</v>
+      </c>
+      <c r="F46" s="1">
+        <v>100</v>
+      </c>
+      <c r="G46" s="1">
+        <v>100</v>
+      </c>
+      <c r="H46" s="1">
+        <v>100</v>
+      </c>
+      <c r="I46" s="1">
+        <v>100</v>
+      </c>
+      <c r="J46" s="1">
+        <v>100</v>
+      </c>
+      <c r="K46" s="1">
+        <v>100</v>
+      </c>
       <c r="L46" s="1"/>
       <c r="M46" s="2" t="s">
         <v>26</v>
@@ -3588,14 +4787,30 @@
       <c r="C47" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
+      <c r="D47" s="1">
+        <v>100</v>
+      </c>
+      <c r="E47" s="1">
+        <v>100</v>
+      </c>
+      <c r="F47" s="1">
+        <v>100</v>
+      </c>
+      <c r="G47" s="1">
+        <v>100</v>
+      </c>
+      <c r="H47" s="1">
+        <v>100</v>
+      </c>
+      <c r="I47" s="1">
+        <v>100</v>
+      </c>
+      <c r="J47" s="1">
+        <v>100</v>
+      </c>
+      <c r="K47" s="1">
+        <v>100</v>
+      </c>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
@@ -3756,14 +4971,30 @@
       <c r="C52" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
+      <c r="D52" s="1">
+        <v>2</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
+      </c>
+      <c r="G52" s="1">
+        <v>2</v>
+      </c>
+      <c r="H52" s="1">
+        <v>2</v>
+      </c>
+      <c r="I52" s="1">
+        <v>2</v>
+      </c>
+      <c r="J52" s="1">
+        <v>2</v>
+      </c>
+      <c r="K52" s="1">
+        <v>2</v>
+      </c>
       <c r="L52" s="1"/>
       <c r="M52" s="2" t="s">
         <v>32</v>
@@ -3790,14 +5021,30 @@
       <c r="C53" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
+      <c r="D53" s="1">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3</v>
+      </c>
+      <c r="F53" s="1">
+        <v>3</v>
+      </c>
+      <c r="G53" s="1">
+        <v>3</v>
+      </c>
+      <c r="H53" s="1">
+        <v>3</v>
+      </c>
+      <c r="I53" s="1">
+        <v>3</v>
+      </c>
+      <c r="J53" s="1">
+        <v>3</v>
+      </c>
+      <c r="K53" s="1">
+        <v>3</v>
+      </c>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
@@ -3822,14 +5069,30 @@
       <c r="C54" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
+      <c r="D54" s="1">
+        <v>4</v>
+      </c>
+      <c r="E54" s="1">
+        <v>4</v>
+      </c>
+      <c r="F54" s="1">
+        <v>4</v>
+      </c>
+      <c r="G54" s="1">
+        <v>4</v>
+      </c>
+      <c r="H54" s="1">
+        <v>4</v>
+      </c>
+      <c r="I54" s="1">
+        <v>4</v>
+      </c>
+      <c r="J54" s="1">
+        <v>4</v>
+      </c>
+      <c r="K54" s="1">
+        <v>4</v>
+      </c>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
@@ -3854,14 +5117,30 @@
       <c r="C55" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
+      <c r="D55" s="1">
+        <v>5</v>
+      </c>
+      <c r="E55" s="1">
+        <v>5</v>
+      </c>
+      <c r="F55" s="1">
+        <v>5</v>
+      </c>
+      <c r="G55" s="1">
+        <v>5</v>
+      </c>
+      <c r="H55" s="1">
+        <v>5</v>
+      </c>
+      <c r="I55" s="1">
+        <v>5</v>
+      </c>
+      <c r="J55" s="1">
+        <v>5</v>
+      </c>
+      <c r="K55" s="1">
+        <v>5</v>
+      </c>
       <c r="L55" s="1"/>
       <c r="M55" s="2" t="s">
         <v>36</v>
@@ -3888,14 +5167,30 @@
       <c r="C56" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
+      <c r="D56" s="1">
+        <v>6</v>
+      </c>
+      <c r="E56" s="1">
+        <v>6</v>
+      </c>
+      <c r="F56" s="1">
+        <v>6</v>
+      </c>
+      <c r="G56" s="1">
+        <v>6</v>
+      </c>
+      <c r="H56" s="1">
+        <v>6</v>
+      </c>
+      <c r="I56" s="1">
+        <v>6</v>
+      </c>
+      <c r="J56" s="1">
+        <v>6</v>
+      </c>
+      <c r="K56" s="1">
+        <v>6</v>
+      </c>
       <c r="L56" s="1"/>
       <c r="M56" s="2" t="s">
         <v>38</v>
@@ -3922,14 +5217,30 @@
       <c r="C57" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
+      <c r="D57" s="1">
+        <v>7</v>
+      </c>
+      <c r="E57" s="1">
+        <v>7</v>
+      </c>
+      <c r="F57" s="1">
+        <v>7</v>
+      </c>
+      <c r="G57" s="1">
+        <v>7</v>
+      </c>
+      <c r="H57" s="1">
+        <v>7</v>
+      </c>
+      <c r="I57" s="1">
+        <v>7</v>
+      </c>
+      <c r="J57" s="1">
+        <v>7</v>
+      </c>
+      <c r="K57" s="1">
+        <v>7</v>
+      </c>
       <c r="L57" s="1"/>
       <c r="M57" s="2" t="s">
         <v>40</v>
@@ -3956,14 +5267,30 @@
       <c r="C58" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
+      <c r="D58" s="1">
+        <v>8</v>
+      </c>
+      <c r="E58" s="1">
+        <v>8</v>
+      </c>
+      <c r="F58" s="1">
+        <v>8</v>
+      </c>
+      <c r="G58" s="1">
+        <v>8</v>
+      </c>
+      <c r="H58" s="1">
+        <v>8</v>
+      </c>
+      <c r="I58" s="1">
+        <v>8</v>
+      </c>
+      <c r="J58" s="1">
+        <v>8</v>
+      </c>
+      <c r="K58" s="1">
+        <v>8</v>
+      </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
       <c r="N58" s="1"/>
@@ -3988,14 +5315,30 @@
       <c r="C59" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
+      <c r="D59" s="1">
+        <v>9</v>
+      </c>
+      <c r="E59" s="1">
+        <v>9</v>
+      </c>
+      <c r="F59" s="1">
+        <v>9</v>
+      </c>
+      <c r="G59" s="1">
+        <v>9</v>
+      </c>
+      <c r="H59" s="1">
+        <v>9</v>
+      </c>
+      <c r="I59" s="1">
+        <v>9</v>
+      </c>
+      <c r="J59" s="1">
+        <v>9</v>
+      </c>
+      <c r="K59" s="1">
+        <v>9</v>
+      </c>
       <c r="L59" s="1"/>
       <c r="M59" s="2" t="s">
         <v>43</v>
@@ -4022,14 +5365,30 @@
       <c r="C60" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
+      <c r="D60" s="1">
+        <v>10</v>
+      </c>
+      <c r="E60" s="1">
+        <v>10</v>
+      </c>
+      <c r="F60" s="1">
+        <v>10</v>
+      </c>
+      <c r="G60" s="1">
+        <v>10</v>
+      </c>
+      <c r="H60" s="1">
+        <v>10</v>
+      </c>
+      <c r="I60" s="1">
+        <v>10</v>
+      </c>
+      <c r="J60" s="1">
+        <v>10</v>
+      </c>
+      <c r="K60" s="1">
+        <v>10</v>
+      </c>
       <c r="L60" s="1"/>
       <c r="M60" s="2" t="s">
         <v>45</v>
@@ -4056,14 +5415,30 @@
       <c r="C61" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
+      <c r="D61" s="1">
+        <v>11</v>
+      </c>
+      <c r="E61" s="1">
+        <v>11</v>
+      </c>
+      <c r="F61" s="1">
+        <v>11</v>
+      </c>
+      <c r="G61" s="1">
+        <v>11</v>
+      </c>
+      <c r="H61" s="1">
+        <v>11</v>
+      </c>
+      <c r="I61" s="1">
+        <v>11</v>
+      </c>
+      <c r="J61" s="1">
+        <v>11</v>
+      </c>
+      <c r="K61" s="1">
+        <v>11</v>
+      </c>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
       <c r="N61" s="1"/>
@@ -4088,14 +5463,30 @@
       <c r="C62" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
+      <c r="D62" s="1">
+        <v>12</v>
+      </c>
+      <c r="E62" s="1">
+        <v>12</v>
+      </c>
+      <c r="F62" s="1">
+        <v>12</v>
+      </c>
+      <c r="G62" s="1">
+        <v>12</v>
+      </c>
+      <c r="H62" s="1">
+        <v>12</v>
+      </c>
+      <c r="I62" s="1">
+        <v>12</v>
+      </c>
+      <c r="J62" s="1">
+        <v>12</v>
+      </c>
+      <c r="K62" s="1">
+        <v>12</v>
+      </c>
       <c r="L62" s="1"/>
       <c r="M62" s="2" t="s">
         <v>48</v>
@@ -4122,14 +5513,30 @@
       <c r="C63" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
+      <c r="D63" s="1">
+        <v>13</v>
+      </c>
+      <c r="E63" s="1">
+        <v>13</v>
+      </c>
+      <c r="F63" s="1">
+        <v>13</v>
+      </c>
+      <c r="G63" s="1">
+        <v>13</v>
+      </c>
+      <c r="H63" s="1">
+        <v>13</v>
+      </c>
+      <c r="I63" s="1">
+        <v>13</v>
+      </c>
+      <c r="J63" s="1">
+        <v>13</v>
+      </c>
+      <c r="K63" s="1">
+        <v>13</v>
+      </c>
       <c r="L63" s="1"/>
       <c r="M63" s="2" t="s">
         <v>50</v>
@@ -4156,14 +5563,30 @@
       <c r="C64" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
+      <c r="D64" s="1">
+        <v>14</v>
+      </c>
+      <c r="E64" s="1">
+        <v>14</v>
+      </c>
+      <c r="F64" s="1">
+        <v>14</v>
+      </c>
+      <c r="G64" s="1">
+        <v>14</v>
+      </c>
+      <c r="H64" s="1">
+        <v>14</v>
+      </c>
+      <c r="I64" s="1">
+        <v>14</v>
+      </c>
+      <c r="J64" s="1">
+        <v>14</v>
+      </c>
+      <c r="K64" s="1">
+        <v>14</v>
+      </c>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
       <c r="N64" s="1"/>
@@ -4188,14 +5611,30 @@
       <c r="C65" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
+      <c r="D65" s="1">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1">
+        <v>15</v>
+      </c>
+      <c r="F65" s="1">
+        <v>15</v>
+      </c>
+      <c r="G65" s="1">
+        <v>15</v>
+      </c>
+      <c r="H65" s="1">
+        <v>15</v>
+      </c>
+      <c r="I65" s="1">
+        <v>15</v>
+      </c>
+      <c r="J65" s="1">
+        <v>15</v>
+      </c>
+      <c r="K65" s="1">
+        <v>15</v>
+      </c>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
       <c r="N65" s="1"/>
@@ -4220,14 +5659,30 @@
       <c r="C66" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
+      <c r="D66" s="1">
+        <v>16</v>
+      </c>
+      <c r="E66" s="1">
+        <v>16</v>
+      </c>
+      <c r="F66" s="1">
+        <v>16</v>
+      </c>
+      <c r="G66" s="1">
+        <v>16</v>
+      </c>
+      <c r="H66" s="1">
+        <v>16</v>
+      </c>
+      <c r="I66" s="1">
+        <v>16</v>
+      </c>
+      <c r="J66" s="1">
+        <v>16</v>
+      </c>
+      <c r="K66" s="1">
+        <v>16</v>
+      </c>
       <c r="L66" s="1"/>
       <c r="M66" s="2" t="s">
         <v>89</v>
@@ -4254,14 +5709,30 @@
       <c r="C67" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
+      <c r="D67" s="1">
+        <v>17</v>
+      </c>
+      <c r="E67" s="1">
+        <v>17</v>
+      </c>
+      <c r="F67" s="1">
+        <v>17</v>
+      </c>
+      <c r="G67" s="1">
+        <v>17</v>
+      </c>
+      <c r="H67" s="1">
+        <v>17</v>
+      </c>
+      <c r="I67" s="1">
+        <v>17</v>
+      </c>
+      <c r="J67" s="1">
+        <v>17</v>
+      </c>
+      <c r="K67" s="1">
+        <v>17</v>
+      </c>
       <c r="L67" s="1"/>
       <c r="M67" s="2" t="s">
         <v>90</v>
@@ -4288,14 +5759,30 @@
       <c r="C68" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
+      <c r="D68" s="1">
+        <v>18</v>
+      </c>
+      <c r="E68" s="1">
+        <v>18</v>
+      </c>
+      <c r="F68" s="1">
+        <v>18</v>
+      </c>
+      <c r="G68" s="1">
+        <v>18</v>
+      </c>
+      <c r="H68" s="1">
+        <v>18</v>
+      </c>
+      <c r="I68" s="1">
+        <v>18</v>
+      </c>
+      <c r="J68" s="1">
+        <v>18</v>
+      </c>
+      <c r="K68" s="1">
+        <v>18</v>
+      </c>
       <c r="L68" s="1"/>
       <c r="M68" s="1" t="s">
         <v>99</v>
@@ -4322,14 +5809,30 @@
       <c r="C69" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
+      <c r="D69" s="1">
+        <v>19</v>
+      </c>
+      <c r="E69" s="1">
+        <v>19</v>
+      </c>
+      <c r="F69" s="1">
+        <v>19</v>
+      </c>
+      <c r="G69" s="1">
+        <v>19</v>
+      </c>
+      <c r="H69" s="1">
+        <v>19</v>
+      </c>
+      <c r="I69" s="1">
+        <v>19</v>
+      </c>
+      <c r="J69" s="1">
+        <v>19</v>
+      </c>
+      <c r="K69" s="1">
+        <v>19</v>
+      </c>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
@@ -4354,14 +5857,30 @@
       <c r="C70" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
+      <c r="D70" s="1">
+        <v>20</v>
+      </c>
+      <c r="E70" s="1">
+        <v>20</v>
+      </c>
+      <c r="F70" s="1">
+        <v>20</v>
+      </c>
+      <c r="G70" s="1">
+        <v>20</v>
+      </c>
+      <c r="H70" s="1">
+        <v>20</v>
+      </c>
+      <c r="I70" s="1">
+        <v>20</v>
+      </c>
+      <c r="J70" s="1">
+        <v>20</v>
+      </c>
+      <c r="K70" s="1">
+        <v>20</v>
+      </c>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
@@ -4386,14 +5905,30 @@
       <c r="C71" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
+      <c r="D71" s="1">
+        <v>21</v>
+      </c>
+      <c r="E71" s="1">
+        <v>21</v>
+      </c>
+      <c r="F71" s="1">
+        <v>21</v>
+      </c>
+      <c r="G71" s="1">
+        <v>21</v>
+      </c>
+      <c r="H71" s="1">
+        <v>21</v>
+      </c>
+      <c r="I71" s="1">
+        <v>21</v>
+      </c>
+      <c r="J71" s="1">
+        <v>21</v>
+      </c>
+      <c r="K71" s="1">
+        <v>21</v>
+      </c>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
       <c r="N71" s="1"/>
@@ -4418,14 +5953,30 @@
       <c r="C72" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
+      <c r="D72" s="1">
+        <v>22</v>
+      </c>
+      <c r="E72" s="1">
+        <v>22</v>
+      </c>
+      <c r="F72" s="1">
+        <v>22</v>
+      </c>
+      <c r="G72" s="1">
+        <v>22</v>
+      </c>
+      <c r="H72" s="1">
+        <v>22</v>
+      </c>
+      <c r="I72" s="1">
+        <v>22</v>
+      </c>
+      <c r="J72" s="1">
+        <v>22</v>
+      </c>
+      <c r="K72" s="1">
+        <v>22</v>
+      </c>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
       <c r="N72" s="1"/>
@@ -4450,14 +6001,30 @@
       <c r="C73" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
+      <c r="D73" s="1">
+        <v>23</v>
+      </c>
+      <c r="E73" s="1">
+        <v>23</v>
+      </c>
+      <c r="F73" s="1">
+        <v>23</v>
+      </c>
+      <c r="G73" s="1">
+        <v>23</v>
+      </c>
+      <c r="H73" s="1">
+        <v>23</v>
+      </c>
+      <c r="I73" s="1">
+        <v>23</v>
+      </c>
+      <c r="J73" s="1">
+        <v>23</v>
+      </c>
+      <c r="K73" s="1">
+        <v>23</v>
+      </c>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
       <c r="N73" s="1"/>
@@ -4482,14 +6049,30 @@
       <c r="C74" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
+      <c r="D74" s="1">
+        <v>24</v>
+      </c>
+      <c r="E74" s="1">
+        <v>24</v>
+      </c>
+      <c r="F74" s="1">
+        <v>24</v>
+      </c>
+      <c r="G74" s="1">
+        <v>24</v>
+      </c>
+      <c r="H74" s="1">
+        <v>24</v>
+      </c>
+      <c r="I74" s="1">
+        <v>24</v>
+      </c>
+      <c r="J74" s="1">
+        <v>24</v>
+      </c>
+      <c r="K74" s="1">
+        <v>24</v>
+      </c>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
       <c r="N74" s="1"/>
@@ -4514,14 +6097,30 @@
       <c r="C75" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
+      <c r="D75" s="1">
+        <v>25</v>
+      </c>
+      <c r="E75" s="1">
+        <v>25</v>
+      </c>
+      <c r="F75" s="1">
+        <v>25</v>
+      </c>
+      <c r="G75" s="1">
+        <v>25</v>
+      </c>
+      <c r="H75" s="1">
+        <v>25</v>
+      </c>
+      <c r="I75" s="1">
+        <v>25</v>
+      </c>
+      <c r="J75" s="1">
+        <v>25</v>
+      </c>
+      <c r="K75" s="1">
+        <v>25</v>
+      </c>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
       <c r="N75" s="1"/>
@@ -4546,14 +6145,30 @@
       <c r="C76" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
+      <c r="D76" s="1">
+        <v>26</v>
+      </c>
+      <c r="E76" s="1">
+        <v>26</v>
+      </c>
+      <c r="F76" s="1">
+        <v>26</v>
+      </c>
+      <c r="G76" s="1">
+        <v>26</v>
+      </c>
+      <c r="H76" s="1">
+        <v>26</v>
+      </c>
+      <c r="I76" s="1">
+        <v>26</v>
+      </c>
+      <c r="J76" s="1">
+        <v>26</v>
+      </c>
+      <c r="K76" s="1">
+        <v>26</v>
+      </c>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
       <c r="N76" s="1"/>
@@ -4578,14 +6193,30 @@
       <c r="C77" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
+      <c r="D77" s="1">
+        <v>27</v>
+      </c>
+      <c r="E77" s="1">
+        <v>27</v>
+      </c>
+      <c r="F77" s="1">
+        <v>27</v>
+      </c>
+      <c r="G77" s="1">
+        <v>27</v>
+      </c>
+      <c r="H77" s="1">
+        <v>27</v>
+      </c>
+      <c r="I77" s="1">
+        <v>27</v>
+      </c>
+      <c r="J77" s="1">
+        <v>27</v>
+      </c>
+      <c r="K77" s="1">
+        <v>27</v>
+      </c>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
       <c r="N77" s="1"/>
@@ -4610,14 +6241,30 @@
       <c r="C78" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
+      <c r="D78" s="1">
+        <v>28</v>
+      </c>
+      <c r="E78" s="1">
+        <v>28</v>
+      </c>
+      <c r="F78" s="1">
+        <v>28</v>
+      </c>
+      <c r="G78" s="1">
+        <v>28</v>
+      </c>
+      <c r="H78" s="1">
+        <v>28</v>
+      </c>
+      <c r="I78" s="1">
+        <v>28</v>
+      </c>
+      <c r="J78" s="1">
+        <v>28</v>
+      </c>
+      <c r="K78" s="1">
+        <v>28</v>
+      </c>
       <c r="L78" s="1"/>
       <c r="M78" s="1"/>
       <c r="N78" s="1"/>
@@ -4642,14 +6289,30 @@
       <c r="C79" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
+      <c r="D79" s="1">
+        <v>29</v>
+      </c>
+      <c r="E79" s="1">
+        <v>29</v>
+      </c>
+      <c r="F79" s="1">
+        <v>29</v>
+      </c>
+      <c r="G79" s="1">
+        <v>29</v>
+      </c>
+      <c r="H79" s="1">
+        <v>29</v>
+      </c>
+      <c r="I79" s="1">
+        <v>29</v>
+      </c>
+      <c r="J79" s="1">
+        <v>29</v>
+      </c>
+      <c r="K79" s="1">
+        <v>29</v>
+      </c>
       <c r="L79" s="1"/>
       <c r="M79" s="1"/>
       <c r="N79" s="1"/>
@@ -4674,14 +6337,30 @@
       <c r="C80" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
+      <c r="D80" s="1">
+        <v>30</v>
+      </c>
+      <c r="E80" s="1">
+        <v>30</v>
+      </c>
+      <c r="F80" s="1">
+        <v>30</v>
+      </c>
+      <c r="G80" s="1">
+        <v>30</v>
+      </c>
+      <c r="H80" s="1">
+        <v>30</v>
+      </c>
+      <c r="I80" s="1">
+        <v>30</v>
+      </c>
+      <c r="J80" s="1">
+        <v>30</v>
+      </c>
+      <c r="K80" s="1">
+        <v>30</v>
+      </c>
       <c r="L80" s="1"/>
       <c r="M80" s="1"/>
       <c r="N80" s="1"/>
@@ -4706,14 +6385,30 @@
       <c r="C81" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
+      <c r="D81" s="1">
+        <v>31</v>
+      </c>
+      <c r="E81" s="1">
+        <v>31</v>
+      </c>
+      <c r="F81" s="1">
+        <v>31</v>
+      </c>
+      <c r="G81" s="1">
+        <v>31</v>
+      </c>
+      <c r="H81" s="1">
+        <v>31</v>
+      </c>
+      <c r="I81" s="1">
+        <v>31</v>
+      </c>
+      <c r="J81" s="1">
+        <v>31</v>
+      </c>
+      <c r="K81" s="1">
+        <v>31</v>
+      </c>
       <c r="L81" s="1"/>
       <c r="M81" s="1"/>
       <c r="N81" s="1"/>

</xml_diff>

<commit_message>
Update tools - Kingdom Simulator
</commit_message>
<xml_diff>
--- a/Kingdom/KingdomSimulator.xlsx
+++ b/Kingdom/KingdomSimulator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/Kingdom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD23B53-EB47-884B-8344-F631017C9F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A171CF93-1587-2B45-A008-85C2038AA162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-1040" yWindow="-21100" windowWidth="36060" windowHeight="19800" xr2:uid="{7FFFBABC-6793-4F48-8984-0BF1F567D385}"/>
   </bookViews>
@@ -370,7 +370,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -397,6 +397,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="苹方-简"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="苹方-简"/>
       <family val="2"/>
     </font>
@@ -457,29 +463,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -793,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1008FC5-4C04-EE4B-A35B-C84E380B5767}">
   <dimension ref="A1:BC1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -803,40 +812,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:55">
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="10"/>
-      <c r="AZ1" s="10"/>
-      <c r="BA1" s="10"/>
-      <c r="BB1" s="10"/>
-      <c r="BC1" s="10"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7"/>
+      <c r="AS1" s="7"/>
+      <c r="AT1" s="7"/>
+      <c r="AU1" s="7"/>
+      <c r="AV1" s="7"/>
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7"/>
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="7"/>
     </row>
     <row r="2" spans="1:55">
       <c r="A2" s="1"/>
@@ -910,11 +919,11 @@
         <v>5</v>
       </c>
       <c r="R3" s="1"/>
-      <c r="S3" s="1">
-        <v>2</v>
+      <c r="S3">
+        <v>1</v>
       </c>
       <c r="T3" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="2" t="s">
@@ -967,11 +976,11 @@
         <v>5</v>
       </c>
       <c r="R4" s="1"/>
-      <c r="S4" s="2">
-        <v>3</v>
-      </c>
-      <c r="T4" s="2">
-        <v>6</v>
+      <c r="S4" s="1">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1">
+        <v>4</v>
       </c>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -985,28 +994,28 @@
       <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="11">
         <v>0.5</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="12">
         <v>0.38938842346886499</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="12">
         <v>0.23240303306998999</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="12">
         <v>0.121077935222672</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="12">
         <v>5.4166666666666599E-2</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="13">
         <v>1.694915E-2</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="12">
         <v>0</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="12">
         <v>0</v>
       </c>
       <c r="L5" s="1"/>
@@ -1022,17 +1031,17 @@
         <v>5</v>
       </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="1">
-        <v>4</v>
-      </c>
-      <c r="T5" s="1">
-        <v>8</v>
+      <c r="S5" s="2">
+        <v>3</v>
+      </c>
+      <c r="T5" s="2">
+        <v>6</v>
       </c>
       <c r="U5" s="2"/>
-      <c r="V5" s="11" t="s">
+      <c r="V5" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="W5" s="12"/>
+      <c r="W5" s="9"/>
       <c r="X5" t="s">
         <v>72</v>
       </c>
@@ -1135,28 +1144,28 @@
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="12">
         <v>0.61061157653113396</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="11">
         <v>0.5</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="12">
         <v>0.31754829433454601</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="12">
         <v>0.19900250614128601</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="12">
         <v>0.110471929263875</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="12">
         <v>6.6095471236230094E-2</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="12">
         <v>0</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="12">
         <v>0</v>
       </c>
       <c r="L6" s="1"/>
@@ -1173,13 +1182,13 @@
       </c>
       <c r="R6" s="1"/>
       <c r="S6" s="1">
-        <v>5</v>
-      </c>
-      <c r="T6" s="2">
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="T6" s="1">
+        <v>8</v>
       </c>
       <c r="U6" s="2"/>
-      <c r="V6" s="13" t="s">
+      <c r="V6" s="10" t="s">
         <v>102</v>
       </c>
       <c r="W6" t="s">
@@ -1287,28 +1296,28 @@
       <c r="C7" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="12">
         <v>0.76759696693000901</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="12">
         <v>0.68246330094385499</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="11">
         <v>0.5</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="12">
         <v>0.34141425942693499</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="12">
         <v>0.208795117211068</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="12">
         <v>0.13136309825807499</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="12">
         <v>0.110878661087866</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="14">
         <v>0</v>
       </c>
       <c r="L7" s="1"/>
@@ -1325,10 +1334,10 @@
       </c>
       <c r="R7" s="1"/>
       <c r="S7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="T7" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="U7" s="2"/>
       <c r="V7" s="1"/>
@@ -1437,28 +1446,28 @@
       <c r="C8" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="14">
         <v>0.87892206477732704</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="14">
         <v>0.80099749385871299</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="11">
         <v>0.65858574057306396</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="11">
         <v>0.5</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="14">
         <v>0.344536205929314</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="14">
         <v>0.23573049055241099</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="14">
         <v>0.18038875820230199</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="14">
         <v>0.13207547169811301</v>
       </c>
       <c r="L8" s="1"/>
@@ -1474,8 +1483,12 @@
         <v>7</v>
       </c>
       <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
+      <c r="S8" s="1">
+        <v>6</v>
+      </c>
+      <c r="T8" s="2">
+        <v>12</v>
+      </c>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1" t="s">
@@ -1583,28 +1596,28 @@
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="14">
         <v>0.94583333333333297</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="14">
         <v>0.88952807073612405</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="14">
         <v>0.79121123397120297</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="11">
         <v>0.65546918827946299</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="11">
         <v>0.5</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="14">
         <v>0.377998789108143</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="14">
         <v>0.28011737216758098</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="14">
         <v>0.21099960901863599</v>
       </c>
       <c r="L9" s="1"/>
@@ -1633,28 +1646,28 @@
       <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="14">
         <v>0.98305084745762705</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="14">
         <v>0.93390452876376895</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="14">
         <v>0.86863690174192398</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="14">
         <v>0.76426950944758798</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="11">
         <v>0.622001210891856</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="11">
         <v>0.50000215074114496</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="14">
         <v>0.38515353228381599</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="14">
         <v>0.28977450007091099</v>
       </c>
       <c r="L10" s="1"/>
@@ -1683,28 +1696,28 @@
       <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="14">
         <v>1</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="14">
         <v>1</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="14">
         <v>0.88912133891213296</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="14">
         <v>0.81961124179769695</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="14">
         <v>0.71988262783241797</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="11">
         <v>0.61484646771618301</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="11">
         <v>0.5</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="14">
         <v>0.40629673356946</v>
       </c>
       <c r="L11" s="1"/>
@@ -1827,28 +1840,28 @@
       <c r="C12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="14">
         <v>1</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="14">
         <v>1</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="14">
         <v>0.70833333333333304</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="14">
         <v>0.86792452830188604</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="14">
         <v>0.78900039098136299</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="14">
         <v>0.71022549992908801</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="11">
         <v>0.59370326643053895</v>
       </c>
-      <c r="K12" s="6">
+      <c r="K12" s="11">
         <v>0.5</v>
       </c>
       <c r="L12" s="1"/>
@@ -2096,19 +2109,19 @@
     <row r="14" spans="1:55">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>

</xml_diff>

<commit_message>
Update tools   Kingdom simulator
</commit_message>
<xml_diff>
--- a/Kingdom/KingdomSimulator.xlsx
+++ b/Kingdom/KingdomSimulator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/Kingdom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A171CF93-1587-2B45-A008-85C2038AA162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D847B47-63B1-564C-B5A1-ED41F36DD120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1040" yWindow="-21100" windowWidth="36060" windowHeight="19800" xr2:uid="{7FFFBABC-6793-4F48-8984-0BF1F567D385}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18940" xr2:uid="{7FFFBABC-6793-4F48-8984-0BF1F567D385}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1008FC5-4C04-EE4B-A35B-C84E380B5767}">
   <dimension ref="A1:BC1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="88" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>

</xml_diff>